<commit_message>
[IMP] Adjust template CD Receivabl Planning
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_planning.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_planning.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Receivable CD Planning Report" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Receivable CD Planning Detail Report" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Receivable CD Planning Detail Report" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -62,16 +62,16 @@
     <t xml:space="preserve">Fiscal Year</t>
   </si>
   <si>
-    <t xml:space="preserve">Quater 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quater 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quater 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quater 4</t>
+    <t xml:space="preserve">Quarter 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quarter 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quarter 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quarter 4</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>

</xml_diff>

<commit_message>
[IMP] Add sla receipt report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_planning.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_planning.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Receivable CD Planning Report" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Receivable CD Planning Detail Report" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Receivable CD Planning Detail Report" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -128,7 +128,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +139,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCFF"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFF0"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -176,7 +182,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -205,7 +211,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -225,7 +235,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,6 +256,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFF0"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -274,80 +352,80 @@
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="7"/>
     </row>
     <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="7"/>
     </row>
     <row r="9" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="7"/>
     </row>
     <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="8"/>
     </row>
     <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+    <row r="12" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -375,10 +453,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="30.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="22.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="29.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="22.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="28.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="20.83"/>
@@ -404,65 +482,65 @@
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="7"/>
       <c r="D4" s="0"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="0"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="15"/>
     </row>
     <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="7"/>
       <c r="D7" s="0"/>
     </row>
     <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="7"/>
       <c r="D8" s="0"/>
     </row>
     <row r="9" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="7"/>
       <c r="D9" s="0"/>
     </row>
     <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="8"/>
       <c r="D10" s="0"/>
     </row>
     <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,35 +549,35 @@
       <c r="C11" s="0"/>
       <c r="D11" s="0"/>
     </row>
-    <row r="12" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+    <row r="12" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="9" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[IMP] Adjust CD Receivable Planning
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_planning.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_planning.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Receivable CD Planning Report" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Receivable CD Planning Detail Report" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Receivable CD Planning Detail Report" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -93,10 +93,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00_);\(#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="#,###.00"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -182,7 +183,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -232,6 +233,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,6 +261,18 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -430,6 +447,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:F1048576">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>IF($A1="Total",TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -458,10 +480,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="24.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="13" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="13" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="13" width="24.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="13" width="24.87"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="3" width="11.52"/>
   </cols>
   <sheetData>
@@ -486,7 +508,7 @@
       <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
@@ -503,7 +525,7 @@
       <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -513,7 +535,7 @@
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="15"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">

</xml_diff>

<commit_message>
update Allowance for doubtful accounts Report 13/07/2018
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_planning.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_planning.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Receivable CD Planning Report" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Receivable CD Planning Detail Report" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Receivable CD Planning Detail Report" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -93,10 +93,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00_);\(#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="#,###.00"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -182,7 +183,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -232,6 +233,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,6 +261,18 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -430,6 +447,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:F1048576">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>IF($A1="Total",TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -458,10 +480,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="24.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="13" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="13" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="13" width="24.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="13" width="24.87"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="3" width="11.52"/>
   </cols>
   <sheetData>
@@ -486,7 +508,7 @@
       <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
@@ -503,7 +525,7 @@
       <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -513,7 +535,7 @@
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="15"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">

</xml_diff>

<commit_message>
[IMP] Adjust CD Receivable Planning Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_planning.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cd_receivable_planning.xlsx
@@ -93,11 +93,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,###.00"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -183,7 +182,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,16 +235,12 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -480,10 +475,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="13" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="13" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="13" width="24.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="13" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="24.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="24.87"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="3" width="11.52"/>
   </cols>
   <sheetData>
@@ -492,6 +487,7 @@
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -525,7 +521,7 @@
       <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -535,7 +531,7 @@
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="15"/>
     </row>
     <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">

</xml_diff>